<commit_message>
Projektabschnitt 5: - Informationen Aufgabenblatt exercise_sheet.html  erweitert - Aufgaben werden angezeigt
</commit_message>
<xml_diff>
--- a/Documents/Wochenplan und -bericht/Orga_Wochenplan_KW29.xlsx
+++ b/Documents/Wochenplan und -bericht/Orga_Wochenplan_KW29.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jellef\Documents\GitHub\schoolProject\Documents\Wochenplan und -bericht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792E9AB1-5226-4E0D-88CD-00ED558B75AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959CE0F8-2AC4-4628-A39C-1D24B725F8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3312,7 +3312,7 @@
       <c r="N44" s="28"/>
       <c r="O44" s="28"/>
       <c r="P44" s="23">
-        <v>0.5</v>
+        <v>1.75</v>
       </c>
       <c r="Q44" s="24"/>
       <c r="R44" s="7"/>
@@ -3377,7 +3377,7 @@
       <c r="O47" s="6"/>
       <c r="P47" s="25">
         <f>SUM(P7:R46)</f>
-        <v>29</v>
+        <v>30.25</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>

</xml_diff>